<commit_message>
feat(phase-3.4): Multi-Sheet Excel Import with surrogate keys
- Add migration 002 for product_models_v2 and line_model_compatibilities
- Implement MultiSheetImporter and MultiSheetValidator services
- Add cross-sheet validation for referential integrity
- Refactor compatibilities to use IDs instead of names (Clean Architecture)
- Create SheetSelector, MultiSheetValidationDisplay UI components
- Integrate multi-sheet wizard into ExcelImportPage
- Add 62 passing tests with >80% coverage
- Add test fixture: multi-sheet-production-data.xlsx

Phase 3.4 complete. Ready for Phase 4: Python Integration.
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_lines.xlsx
+++ b/tests/fixtures/test_lines.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>Name</t>
   </si>
@@ -23,9 +23,6 @@
   </si>
   <si>
     <t>Hours Available</t>
-  </si>
-  <si>
-    <t>Efficiency</t>
   </si>
   <si>
     <t>Line X1</t>
@@ -451,7 +448,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -460,7 +457,6 @@
     <col min="1" max="1" style="5" width="13.005" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="5" width="13.005" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="13.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
@@ -473,162 +469,126 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="C2" s="3">
         <v>22</v>
       </c>
-      <c r="D2" s="3">
-        <v>85</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="C3" s="3">
         <v>22</v>
       </c>
-      <c r="D3" s="3">
-        <v>85</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="C4" s="3">
         <v>22</v>
       </c>
-      <c r="D4" s="3">
-        <v>85</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="C5" s="3">
         <v>22</v>
       </c>
-      <c r="D5" s="3">
-        <v>85</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="4">
         <v>22</v>
       </c>
-      <c r="D6" s="4">
-        <v>85</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18">
       <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="C7" s="4">
         <v>20</v>
       </c>
-      <c r="D7" s="4">
-        <v>98</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="4">
         <v>20</v>
       </c>
-      <c r="D8" s="4">
-        <v>98</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="4">
         <v>17</v>
       </c>
-      <c r="D9" s="4">
-        <v>100</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" s="4">
         <v>21</v>
       </c>
-      <c r="D10" s="4">
-        <v>85</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="4">
         <v>21</v>
       </c>
-      <c r="D11" s="4">
-        <v>90</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="3">
         <v>20</v>
-      </c>
-      <c r="D12" s="3">
-        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>